<commit_message>
rename passives, fix silk
</commit_message>
<xml_diff>
--- a/hardware/power_supply_module/rev_d/power_supply_module_bom.xlsx
+++ b/hardware/power_supply_module/rev_d/power_supply_module_bom.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="power_supply_module_bom" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="193">
   <si>
     <t xml:space="preserve">Qty</t>
   </si>
@@ -58,7 +58,7 @@
     <t xml:space="preserve">1727-5151-1-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">0.010 ?</t>
+    <t xml:space="preserve">0.010 Ω</t>
   </si>
   <si>
     <t xml:space="preserve">RESISTOR0805_RES</t>
@@ -76,7 +76,7 @@
     <t xml:space="preserve">WSLPB-.01CT-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">0.017 ?</t>
+    <t xml:space="preserve">0.017 Ω</t>
   </si>
   <si>
     <t xml:space="preserve">R2, R3, R4, R5, R6, R7, R8, R9</t>
@@ -85,7 +85,7 @@
     <t xml:space="preserve">WSLPB-.017CT-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">0.05 ?</t>
+    <t xml:space="preserve">0.05 Ω</t>
   </si>
   <si>
     <t xml:space="preserve">R10, R11</t>
@@ -106,7 +106,7 @@
     <t xml:space="preserve">C1, C2, C3, C4, C5, C6, C7, C8, C9, C10, C11, C12, C13, C14, C15, C16, C17, C18, C19, C20, C21, C22, C23</t>
   </si>
   <si>
-    <t xml:space="preserve">0402 Capacitor</t>
+    <t xml:space="preserve">SMD Capacitor</t>
   </si>
   <si>
     <t xml:space="preserve">490-5920-1-ND </t>
@@ -130,7 +130,7 @@
     <t xml:space="preserve">490-10440-1-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">1 M?</t>
+    <t xml:space="preserve">1 MΩ</t>
   </si>
   <si>
     <t xml:space="preserve">RESISTOR0402_RES</t>
@@ -139,19 +139,28 @@
     <t xml:space="preserve">0402_RES</t>
   </si>
   <si>
+    <t xml:space="preserve">R15, R16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P1.0KJCT-ND</t>
+  </si>
+  <si>
     <t xml:space="preserve">R14</t>
   </si>
   <si>
     <t xml:space="preserve">P1.00MLCT-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">1 k?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R12, R13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P1.0KJCT-ND</t>
+    <t xml:space="preserve">1 kΩ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P150LCT-ND</t>
   </si>
   <si>
     <t xml:space="preserve">1 uF</t>
@@ -184,37 +193,37 @@
     <t xml:space="preserve">490-5523-1-ND </t>
   </si>
   <si>
-    <t xml:space="preserve">100 k?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R43, R44, R45, R46, R47</t>
+    <t xml:space="preserve">100 kΩ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R45, R46, R47, R48, R49</t>
   </si>
   <si>
     <t xml:space="preserve">P100KJCT-ND </t>
   </si>
   <si>
-    <t xml:space="preserve">130 k?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R48, R49, R50, R51</t>
+    <t xml:space="preserve">130 kΩ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R50, R51, R52, R53</t>
   </si>
   <si>
     <t xml:space="preserve">P130KLCT-ND </t>
   </si>
   <si>
-    <t xml:space="preserve">150 ?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R52, R53</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P150LCT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 k?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R15, R16, R17, R18, R19, R20, R21, R22, R23, R24, R25, R26, R27, R28, R29, R30, R31, R32, R33, R34, R35, R36, R37, R38, R39, R40, R41</t>
+    <t xml:space="preserve">150 Ω</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 kΩ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R17, R18, R19, R20, R21, R22, R23, R24, R25, R26, R27, R28, R29, R30, R31, R32, R33, R34, R35, R36, R37, R38, R39, R40, R41, R42, R43</t>
   </si>
   <si>
     <t xml:space="preserve">P2.00KLCT-ND</t>
@@ -247,19 +256,19 @@
     <t xml:space="preserve">1276-1193-1-ND </t>
   </si>
   <si>
-    <t xml:space="preserve">23.2 k?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R42</t>
-  </si>
-  <si>
-    <t xml:space="preserve">311-2257-1-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">240 k?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R54</t>
+    <t xml:space="preserve">23.2 kΩ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P23.2KDATR-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">240 kΩ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R56</t>
   </si>
   <si>
     <t xml:space="preserve">P240KLCT-ND</t>
@@ -289,25 +298,25 @@
     <t xml:space="preserve">Very simple LDO 100ma 3v3</t>
   </si>
   <si>
-    <t xml:space="preserve">LM3480IM3-3.3/NOPBCT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">301 k?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R55</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P301KLCT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">340 k?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R56</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P340KLCT-ND</t>
+    <t xml:space="preserve">ZMR330FCT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">301 kΩ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P301KDATR-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">340 kΩ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P340KDACT-ND</t>
   </si>
   <si>
     <t xml:space="preserve">6.8uH</t>
@@ -325,31 +334,31 @@
     <t xml:space="preserve">541-2582-1-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">680 k?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R57, R58, R59, R60</t>
+    <t xml:space="preserve">680 kΩ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R59, R60, R61, R62</t>
   </si>
   <si>
     <t xml:space="preserve">P680KLCT-ND </t>
   </si>
   <si>
-    <t xml:space="preserve">750 k?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R61</t>
+    <t xml:space="preserve">750 kΩ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R63</t>
   </si>
   <si>
     <t xml:space="preserve">P750KJCT-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">953 k?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R62</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P953KLCT-ND</t>
+    <t xml:space="preserve">953 kΩ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P953KDACT-ND</t>
   </si>
   <si>
     <t xml:space="preserve">AP22814</t>
@@ -367,18 +376,21 @@
     <t xml:space="preserve">AP22814ASN-7DICT-ND</t>
   </si>
   <si>
+    <t xml:space="preserve">DIODE_SCHOTTKYSOD323</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CMDSH2-4L CT-ND</t>
+  </si>
+  <si>
     <t xml:space="preserve">DIODE_SCHOTTKYSOT-23F</t>
   </si>
   <si>
     <t xml:space="preserve">SOT-23F</t>
   </si>
   <si>
-    <t xml:space="preserve">D3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CMDSH2-4L CT-ND</t>
-  </si>
-  <si>
     <t xml:space="preserve">D1</t>
   </si>
   <si>
@@ -427,13 +439,28 @@
     <t xml:space="preserve">LT3652EDD#PBF-ND</t>
   </si>
   <si>
+    <t xml:space="preserve">LTC2941</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DFN-6-2MMX3MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I2C Battery Gas Gauge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LTC2941IDCB#TRMPBFCT-ND</t>
+  </si>
+  <si>
     <t xml:space="preserve">LTC2943</t>
   </si>
   <si>
     <t xml:space="preserve">DFN-8</t>
   </si>
   <si>
-    <t xml:space="preserve">U8, U9, U10, U11, U12, U13, U14, U15, U26</t>
+    <t xml:space="preserve">U9, U10, U11, U12, U13, U14, U15, U26</t>
   </si>
   <si>
     <t xml:space="preserve">Multicell Battery Gas Gauge</t>
@@ -448,7 +475,7 @@
     <t xml:space="preserve">U29</t>
   </si>
   <si>
-    <t xml:space="preserve">1K I2C?"? Serial EEPROM</t>
+    <t xml:space="preserve">1K I2C™ Serial EEPROM</t>
   </si>
   <si>
     <t xml:space="preserve">497-8631-1-ND</t>
@@ -481,9 +508,6 @@
     <t xml:space="preserve">A simple watchdog timer with adjustable timeouts and reset time</t>
   </si>
   <si>
-    <t xml:space="preserve">MAX6746KA26+TCT-ND</t>
-  </si>
-  <si>
     <t xml:space="preserve">MODULE_POWER</t>
   </si>
   <si>
@@ -524,6 +548,30 @@
   </si>
   <si>
     <t xml:space="preserve">296-20960-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PTS810SJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PTS810SJ Push Button Switch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CKN10504CT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC2030-FTDI-I2C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC2030-IDC-NL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UMFT200XD FTDI to I2C pogo pin adapter.</t>
   </si>
   <si>
     <t xml:space="preserve">TE_SSA12/SPDT</t>
@@ -646,21 +694,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:H49"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A48" activeCellId="0" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.28571428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="26.7295918367347"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.734693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="118.071428571429"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="63.3571428571429"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.1887755102041"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.6479591836735"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.47959183673469"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="26.8520408163265"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.0765306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="116.760204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="63.2551020408163"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.719387755102"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.6275510204082"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
@@ -847,7 +895,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>36</v>
@@ -870,10 +918,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>37</v>
@@ -882,13 +930,13 @@
         <v>38</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F10" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -896,99 +944,99 @@
         <v>1</v>
       </c>
       <c r="B11" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>47</v>
-      </c>
       <c r="F11" s="0" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>37</v>
@@ -997,21 +1045,21 @@
         <v>38</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F15" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>37</v>
@@ -1020,67 +1068,67 @@
         <v>38</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F16" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>68</v>
+        <v>38</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>70</v>
+        <v>16</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="D18" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" s="0" t="s">
         <v>46</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="F18" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="G18" s="0" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>37</v>
@@ -1089,59 +1137,59 @@
         <v>38</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="F19" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>16</v>
+        <v>73</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="F21" s="0" t="s">
         <v>28</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1149,22 +1197,22 @@
         <v>1</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>85</v>
+        <v>13</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>86</v>
+        <v>14</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>88</v>
+        <v>16</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1172,7 +1220,7 @@
         <v>1</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>37</v>
@@ -1181,36 +1229,36 @@
         <v>38</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="F23" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1218,45 +1266,45 @@
         <v>1</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="F26" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1264,22 +1312,22 @@
         <v>1</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="F27" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1287,45 +1335,45 @@
         <v>1</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>37</v>
+        <v>100</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>38</v>
+        <v>101</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>16</v>
+        <v>73</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>110</v>
+        <v>37</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>111</v>
+        <v>38</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>113</v>
+        <v>16</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1333,19 +1381,22 @@
         <v>1</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>115</v>
+        <v>37</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>116</v>
+        <v>38</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>117</v>
+        <v>108</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>16</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1353,39 +1404,45 @@
         <v>1</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>115</v>
+        <v>13</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>116</v>
+        <v>14</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>119</v>
+        <v>111</v>
+      </c>
+      <c r="F31" s="0" t="s">
+        <v>16</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>123</v>
+        <v>115</v>
+      </c>
+      <c r="F32" s="0" t="s">
+        <v>116</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1393,22 +1450,19 @@
         <v>1</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>126</v>
+        <v>9</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="F33" s="0" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1416,45 +1470,39 @@
         <v>1</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="F34" s="0" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="F35" s="0" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1462,22 +1510,22 @@
         <v>1</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1485,22 +1533,22 @@
         <v>1</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="H37" s="0" t="s">
-        <v>148</v>
+        <v>137</v>
+      </c>
+      <c r="G37" s="0" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1508,45 +1556,45 @@
         <v>1</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1554,45 +1602,45 @@
         <v>1</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>159</v>
+        <v>130</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="G40" s="0" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>166</v>
-      </c>
-      <c r="G41" s="0" t="s">
-        <v>167</v>
+        <v>156</v>
+      </c>
+      <c r="H41" s="0" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1600,51 +1648,183 @@
         <v>1</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="G42" s="0" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="E43" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="F43" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="G43" s="0" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="E44" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="F44" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="G44" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="E45" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="F45" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="G45" s="0" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="E46" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="F46" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="G46" s="0" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="E47" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="F47" s="0" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="D48" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="E48" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="F48" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="G48" s="0" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="B43" s="0" t="s">
-        <v>172</v>
-      </c>
-      <c r="C43" s="0" t="s">
-        <v>172</v>
-      </c>
-      <c r="D43" s="0" t="s">
-        <v>173</v>
-      </c>
-      <c r="E43" s="0" t="s">
-        <v>174</v>
-      </c>
-      <c r="F43" s="0" t="s">
-        <v>175</v>
-      </c>
-      <c r="G43" s="0" t="s">
-        <v>176</v>
+      <c r="B49" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="D49" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="E49" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="F49" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="G49" s="0" t="s">
+        <v>192</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>